<commit_message>
25/05- Added outlier check and the Price model works as intended
</commit_message>
<xml_diff>
--- a/Reference_annual_2022.xlsx
+++ b/Reference_annual_2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucar\PycharmProjects\NJORD_2022_Albin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51D6C13-E027-49E6-A556-3A78CC751AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0F3D0F-DE7C-4C25-AAB6-B87C848EE976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{897FD0AD-667B-405B-B21E-969CA7E21E5D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="338">
   <si>
     <t>Country</t>
   </si>
@@ -1017,10 +1017,6 @@
     <t>2020 - Total - annual</t>
   </si>
   <si>
-    <t xml:space="preserve">17 944
-</t>
-  </si>
-  <si>
     <t>Faroe Islands</t>
   </si>
   <si>
@@ -1038,12 +1034,27 @@
   <si>
     <t>United States of America</t>
   </si>
+  <si>
+    <t>2021 - Total - annual</t>
+  </si>
+  <si>
+    <t>2021 - IRENA - annual</t>
+  </si>
+  <si>
+    <t>2021 - ITC - annual</t>
+  </si>
+  <si>
+    <t>2021 - PVPS - annual</t>
+  </si>
+  <si>
+    <t>2021 - Other - annual</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1063,6 +1074,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1100,7 +1117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1108,6 +1125,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1422,13 +1440,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9330EB-2987-4E38-92E6-5B4CF5CB713B}">
-  <dimension ref="A1:CX232"/>
+  <dimension ref="A1:DC232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B222" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AT72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A231" sqref="A231"/>
+      <selection pane="bottomRight" activeCell="BA84" sqref="BA84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1436,7 +1454,7 @@
     <col min="1" max="1" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1743,8 +1761,23 @@
       <c r="CX1" t="s">
         <v>326</v>
       </c>
+      <c r="CY1" t="s">
+        <v>334</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>335</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>336</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>337</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>333</v>
+      </c>
     </row>
-    <row r="2" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2052,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2360,7 +2393,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2668,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2976,7 +3009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3284,7 +3317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3592,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3900,7 +3933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4208,7 +4241,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4516,7 +4549,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="11" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4824,7 +4857,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -5132,7 +5165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -5440,7 +5473,7 @@
         <v>4503</v>
       </c>
     </row>
-    <row r="14" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -5748,7 +5781,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="15" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -6056,7 +6089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -22382,7 +22415,7 @@
     </row>
     <row r="69" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -25611,8 +25644,8 @@
       <c r="AX79">
         <v>7440</v>
       </c>
-      <c r="AY79" t="s">
-        <v>327</v>
+      <c r="AY79" s="3">
+        <v>17944</v>
       </c>
       <c r="AZ79">
         <v>7440</v>
@@ -28542,7 +28575,7 @@
     </row>
     <row r="89" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -33470,7 +33503,7 @@
     </row>
     <row r="105" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -57494,7 +57527,7 @@
     </row>
     <row r="183" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -69506,7 +69539,7 @@
     </row>
     <row r="222" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B222">
         <v>0</v>
@@ -69814,7 +69847,7 @@
     </row>
     <row r="223" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -72893,6 +72926,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>